<commit_message>
Validar os cabeçalhos das planilhas
</commit_message>
<xml_diff>
--- a/SME.CDEP.Webapi/Modelos/planilha_acervo_bibliografico.xlsx
+++ b/SME.CDEP.Webapi/Modelos/planilha_acervo_bibliografico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amcomcorp-my.sharepoint.com/personal/vinicius_nyari_amcom_com_br/Documents/CDEP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\SME-CDEP\SME.CDEP.Webapi\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F512F76-96EE-40E0-9E10-AF75CE1D773C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D078D9D-A990-415A-9AAB-FBEC5AEEBDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33285" yWindow="3120" windowWidth="19185" windowHeight="10170" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Acervo Bibliográfico" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Ano</t>
   </si>
   <si>
-    <t>Edicao</t>
-  </si>
-  <si>
     <t>Numero Páginas</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Tombo</t>
+  </si>
+  <si>
+    <t>Edição</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,67 +469,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
       <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrigindo erro de portugês no campo
</commit_message>
<xml_diff>
--- a/SME.CDEP.Webapi/Modelos/planilha_acervo_bibliografico.xlsx
+++ b/SME.CDEP.Webapi/Modelos/planilha_acervo_bibliografico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\SME-CDEP\SME.CDEP.Webapi\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D078D9D-A990-415A-9AAB-FBEC5AEEBDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6BD8C6-1AD1-4A02-A023-71F33E05353B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Acervo Bibliográfico" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Idioma</t>
   </si>
   <si>
-    <t>Localicação CDD</t>
-  </si>
-  <si>
     <t>Localização PHA</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Edição</t>
+  </si>
+  <si>
+    <t>Localização CDD</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,43 +469,43 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
       </c>
       <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
         <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
@@ -517,19 +517,19 @@
         <v>6</v>
       </c>
       <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" t="s">
-        <v>10</v>
-      </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>